<commit_message>
Add expedia tested flow
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Expedia/Data/Config Prod.xlsx
+++ b/Traveloka_DataAutomation_Portal_Expedia/Data/Config Prod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Cybersourcevietin\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793251CC-F6B5-4CAA-8B84-74A4C07C2DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21843E4-05B4-46B0-B476-11ADD75C8A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3852" yWindow="1536" windowWidth="17280" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="672" yWindow="672" windowWidth="17268" windowHeight="8196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
+    <t>FlagError</t>
+  </si>
+  <si>
+    <t>RPA090_Expedia_FlagError</t>
   </si>
 </sst>
 </file>
@@ -618,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -713,7 +719,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2876,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>

</xml_diff>